<commit_message>
Versiones 3040 y 3004
</commit_message>
<xml_diff>
--- a/01.Documentation/Control de versiones de Sistema.xlsx
+++ b/01.Documentation/Control de versiones de Sistema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\01.Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02AC350D-8AAB-4E51-BBC9-C50BDC67E78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53854AA6-42C6-43AD-959E-A7034D0F5B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24CF4CE9-DAD2-45B7-A0D0-75488DFF3356}"/>
+    <workbookView xWindow="-10637" yWindow="9154" windowWidth="22148" windowHeight="13200" xr2:uid="{24CF4CE9-DAD2-45B7-A0D0-75488DFF3356}"/>
   </bookViews>
   <sheets>
     <sheet name="ROVER" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Version</t>
   </si>
@@ -91,9 +91,6 @@
     <t>BOMs</t>
   </si>
   <si>
-    <t>2.0.0</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -107,13 +104,28 @@
   </si>
   <si>
     <t>BOM_DCDC</t>
+  </si>
+  <si>
+    <t>Moficacion Puntual del comparador de la tension de entrada</t>
+  </si>
+  <si>
+    <t>2.0.2</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>2.0.1</t>
+  </si>
+  <si>
+    <t>Modificacion Protocolo de arranque</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +161,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -232,37 +250,39 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,8 +459,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{90806AD9-57A0-44C6-AF8E-190F018DF894}" name="Tabla4" displayName="Tabla4" ref="A2:K8" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A2:K8" xr:uid="{90806AD9-57A0-44C6-AF8E-190F018DF894}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{90806AD9-57A0-44C6-AF8E-190F018DF894}" name="Tabla4" displayName="Tabla4" ref="A2:K12" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A2:K12" xr:uid="{90806AD9-57A0-44C6-AF8E-190F018DF894}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -770,220 +790,360 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O28" sqref="O28"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="K2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="10" t="s">
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3099</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3020</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7">
+        <v>5</v>
+      </c>
+      <c r="J7" s="7">
+        <v>9</v>
+      </c>
+      <c r="K7" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3002</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="7">
+        <v>5</v>
+      </c>
+      <c r="F8" s="7">
+        <v>5</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <v>5</v>
+      </c>
+      <c r="J8" s="7">
+        <v>9</v>
+      </c>
+      <c r="K8" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="39" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3030</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>3000</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3001</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="7">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7">
+        <v>5</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7">
+        <v>5</v>
+      </c>
+      <c r="J9" s="7">
         <v>9</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>3099</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="K9" s="7">
         <v>10</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>9000</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>3010</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="12" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="39" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3003</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="12">
-        <v>5</v>
-      </c>
-      <c r="F7" s="12">
-        <v>5</v>
-      </c>
-      <c r="G7" s="12">
+      <c r="D10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="7">
+        <v>5</v>
+      </c>
+      <c r="F10" s="7">
+        <v>5</v>
+      </c>
+      <c r="G10" s="7">
         <v>2</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H10" s="7">
         <v>1</v>
       </c>
-      <c r="I7" s="12">
-        <v>5</v>
-      </c>
-      <c r="J7" s="12">
+      <c r="I10" s="7">
+        <v>5</v>
+      </c>
+      <c r="J10" s="7">
         <v>9</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K10" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>3002</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="12">
-        <v>5</v>
-      </c>
-      <c r="F8" s="12">
-        <v>5</v>
-      </c>
-      <c r="G8" s="12">
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3040</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="7">
+        <v>5</v>
+      </c>
+      <c r="F11" s="7">
+        <v>5</v>
+      </c>
+      <c r="G11" s="7">
         <v>2</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H11" s="7">
         <v>1</v>
       </c>
-      <c r="I8" s="12">
-        <v>5</v>
-      </c>
-      <c r="J8" s="12">
+      <c r="I11" s="7">
+        <v>5</v>
+      </c>
+      <c r="J11" s="7">
         <v>9</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K11" s="7">
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3004</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="7">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7">
+        <v>5</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7">
+        <v>5</v>
+      </c>
+      <c r="J12" s="7">
+        <v>9</v>
+      </c>
+      <c r="K12" s="7">
+        <v>10</v>
+      </c>
+    </row>
     <row r="25" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Version de Sistema Actualizada
</commit_message>
<xml_diff>
--- a/01.Documentation/Control de versiones de Sistema.xlsx
+++ b/01.Documentation/Control de versiones de Sistema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\01.Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C7121A-4FB4-4FF1-8E3C-4B04FA3B7CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D76DDC9-998F-41D9-9281-56A7AC97A0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24CF4CE9-DAD2-45B7-A0D0-75488DFF3356}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
   <si>
     <t>Cambios</t>
   </si>
@@ -224,6 +224,27 @@
   </si>
   <si>
     <t>3.0.1.0</t>
+  </si>
+  <si>
+    <t>Hotfix Issue 83, salida activada con poca bateria</t>
+  </si>
+  <si>
+    <t>1.2.4</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>2.0.4</t>
+  </si>
+  <si>
+    <t>1.1.3.3</t>
+  </si>
+  <si>
+    <t>3.0.1.1</t>
+  </si>
+  <si>
+    <t>2.0.2.3</t>
   </si>
 </sst>
 </file>
@@ -476,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -528,6 +549,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -564,10 +591,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -887,8 +914,8 @@
   <dimension ref="A1:N99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,56 +938,56 @@
       <c r="A1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -969,36 +996,36 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="29" t="s">
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="28" t="s">
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="23" t="s">
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="25" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="7" t="s">
         <v>27</v>
       </c>
@@ -1032,7 +1059,7 @@
       <c r="M9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="24"/>
+      <c r="N9" s="26"/>
     </row>
     <row r="10" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
@@ -1107,10 +1134,10 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="19" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1158,7 +1185,7 @@
       <c r="E14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="19" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="4">
@@ -1191,10 +1218,10 @@
       <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="19" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1242,7 +1269,7 @@
       <c r="E16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="19" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="4">
@@ -1275,10 +1302,10 @@
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="19" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -1326,7 +1353,7 @@
       <c r="E18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G18" s="4">
@@ -1359,10 +1386,10 @@
       <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="19" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -1410,7 +1437,7 @@
       <c r="E20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="19" t="s">
         <v>40</v>
       </c>
       <c r="G20" s="4">
@@ -1446,7 +1473,7 @@
       <c r="C21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="20" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="6" t="s">
@@ -1485,19 +1512,19 @@
       <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="19">
         <v>6</v>
       </c>
       <c r="H22" s="4">
@@ -1515,7 +1542,7 @@
       <c r="L22" s="4">
         <v>9</v>
       </c>
-      <c r="M22" s="31">
+      <c r="M22" s="19">
         <v>11</v>
       </c>
       <c r="N22" s="11"/>
@@ -1527,19 +1554,19 @@
       <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="D23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="31">
+      <c r="F23" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="19">
         <v>6</v>
       </c>
       <c r="H23" s="4">
@@ -1557,7 +1584,7 @@
       <c r="L23" s="4">
         <v>9</v>
       </c>
-      <c r="M23" s="31">
+      <c r="M23" s="19">
         <v>11</v>
       </c>
       <c r="N23" s="11"/>
@@ -1581,7 +1608,7 @@
       <c r="F24" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="31">
+      <c r="G24" s="19">
         <v>6</v>
       </c>
       <c r="H24" s="4">
@@ -1599,57 +1626,135 @@
       <c r="L24" s="4">
         <v>9</v>
       </c>
-      <c r="M24" s="31">
+      <c r="M24" s="19">
         <v>11</v>
       </c>
       <c r="N24" s="11"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="33">
+        <v>6</v>
+      </c>
+      <c r="H25" s="33">
+        <v>5</v>
+      </c>
+      <c r="I25" s="33">
+        <v>2</v>
+      </c>
+      <c r="J25" s="33">
+        <v>1</v>
+      </c>
+      <c r="K25" s="33">
+        <v>5</v>
+      </c>
+      <c r="L25" s="33">
+        <v>9</v>
+      </c>
+      <c r="M25" s="33">
+        <v>11</v>
+      </c>
       <c r="N25" s="11"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="33">
+        <v>6</v>
+      </c>
+      <c r="H26" s="33">
+        <v>5</v>
+      </c>
+      <c r="I26" s="33">
+        <v>2</v>
+      </c>
+      <c r="J26" s="33">
+        <v>1</v>
+      </c>
+      <c r="K26" s="33">
+        <v>5</v>
+      </c>
+      <c r="L26" s="33">
+        <v>9</v>
+      </c>
+      <c r="M26" s="33">
+        <v>11</v>
+      </c>
       <c r="N26" s="11"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="33">
+        <v>6</v>
+      </c>
+      <c r="H27" s="33">
+        <v>5</v>
+      </c>
+      <c r="I27" s="33">
+        <v>2</v>
+      </c>
+      <c r="J27" s="33">
+        <v>1</v>
+      </c>
+      <c r="K27" s="33">
+        <v>5</v>
+      </c>
+      <c r="L27" s="33">
+        <v>9</v>
+      </c>
+      <c r="M27" s="33">
+        <v>11</v>
+      </c>
       <c r="N27" s="11"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizacion de Contro de versiones
</commit_message>
<xml_diff>
--- a/01.Documentation/Control de versiones de Sistema.xlsx
+++ b/01.Documentation/Control de versiones de Sistema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\01.Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D76DDC9-998F-41D9-9281-56A7AC97A0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E181357-FF07-4F9D-B14A-E6DDEA734B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24CF4CE9-DAD2-45B7-A0D0-75488DFF3356}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="70">
   <si>
     <t>Cambios</t>
   </si>
@@ -245,6 +245,12 @@
   </si>
   <si>
     <t>2.0.2.3</t>
+  </si>
+  <si>
+    <t>Hotfix Issue 80, Modificacion Nitro Cheyenne</t>
+  </si>
+  <si>
+    <t>3.0.1.2</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -589,12 +595,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -915,7 +915,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,34 +1641,34 @@
       <c r="C25" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="33">
+      <c r="G25" s="4">
         <v>6</v>
       </c>
-      <c r="H25" s="33">
-        <v>5</v>
-      </c>
-      <c r="I25" s="33">
+      <c r="H25" s="4">
+        <v>5</v>
+      </c>
+      <c r="I25" s="4">
         <v>2</v>
       </c>
-      <c r="J25" s="33">
+      <c r="J25" s="4">
         <v>1</v>
       </c>
-      <c r="K25" s="33">
-        <v>5</v>
-      </c>
-      <c r="L25" s="33">
+      <c r="K25" s="4">
+        <v>5</v>
+      </c>
+      <c r="L25" s="4">
         <v>9</v>
       </c>
-      <c r="M25" s="33">
+      <c r="M25" s="4">
         <v>11</v>
       </c>
       <c r="N25" s="11"/>
@@ -1680,37 +1680,37 @@
       <c r="B26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G26" s="33">
+      <c r="G26" s="4">
         <v>6</v>
       </c>
-      <c r="H26" s="33">
-        <v>5</v>
-      </c>
-      <c r="I26" s="33">
+      <c r="H26" s="4">
+        <v>5</v>
+      </c>
+      <c r="I26" s="4">
         <v>2</v>
       </c>
-      <c r="J26" s="33">
+      <c r="J26" s="4">
         <v>1</v>
       </c>
-      <c r="K26" s="33">
-        <v>5</v>
-      </c>
-      <c r="L26" s="33">
+      <c r="K26" s="4">
+        <v>5</v>
+      </c>
+      <c r="L26" s="4">
         <v>9</v>
       </c>
-      <c r="M26" s="33">
+      <c r="M26" s="4">
         <v>11</v>
       </c>
       <c r="N26" s="11"/>
@@ -1722,55 +1722,81 @@
       <c r="B27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="34" t="s">
+      <c r="F27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="33">
+      <c r="G27" s="4">
         <v>6</v>
       </c>
-      <c r="H27" s="33">
-        <v>5</v>
-      </c>
-      <c r="I27" s="33">
+      <c r="H27" s="4">
+        <v>5</v>
+      </c>
+      <c r="I27" s="4">
         <v>2</v>
       </c>
-      <c r="J27" s="33">
+      <c r="J27" s="4">
         <v>1</v>
       </c>
-      <c r="K27" s="33">
-        <v>5</v>
-      </c>
-      <c r="L27" s="33">
+      <c r="K27" s="4">
+        <v>5</v>
+      </c>
+      <c r="L27" s="4">
         <v>9</v>
       </c>
-      <c r="M27" s="33">
+      <c r="M27" s="4">
         <v>11</v>
       </c>
       <c r="N27" s="11"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
+    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="4">
+        <v>6</v>
+      </c>
+      <c r="H28" s="4">
+        <v>5</v>
+      </c>
+      <c r="I28" s="4">
+        <v>2</v>
+      </c>
+      <c r="J28" s="4">
+        <v>1</v>
+      </c>
+      <c r="K28" s="4">
+        <v>5</v>
+      </c>
+      <c r="L28" s="4">
+        <v>9</v>
+      </c>
+      <c r="M28" s="4">
+        <v>11</v>
+      </c>
       <c r="N28" s="11"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adiccion del control de software a produccion
</commit_message>
<xml_diff>
--- a/01.Documentation/Control de versiones de Sistema.xlsx
+++ b/01.Documentation/Control de versiones de Sistema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\01.Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E181357-FF07-4F9D-B14A-E6DDEA734B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C15591-2D1B-4A4B-9E61-C711F9AAE26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24CF4CE9-DAD2-45B7-A0D0-75488DFF3356}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24CF4CE9-DAD2-45B7-A0D0-75488DFF3356}"/>
   </bookViews>
   <sheets>
     <sheet name="ROVER" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
   <si>
     <t>Cambios</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>3.0.1.2</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
   </si>
 </sst>
 </file>
@@ -914,8 +917,8 @@
   <dimension ref="A1:N99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
+      <pane ySplit="9" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,7 +1771,7 @@
         <v>14</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Ajuste de control de versiones
</commit_message>
<xml_diff>
--- a/01.Documentation/Control de versiones de Sistema.xlsx
+++ b/01.Documentation/Control de versiones de Sistema.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\01.Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91868FD-BEAB-4D13-AB7D-8F4DA9265BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CC153D-72F8-49DB-917B-39658E7ACD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24CF4CE9-DAD2-45B7-A0D0-75488DFF3356}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{24CF4CE9-DAD2-45B7-A0D0-75488DFF3356}"/>
   </bookViews>
   <sheets>
     <sheet name="ROVER" sheetId="1" r:id="rId1"/>
     <sheet name="TESTs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="76">
   <si>
     <t>Cambios</t>
   </si>
@@ -254,6 +255,21 @@
   </si>
   <si>
     <t>Hotfix Issue 87,85y86.</t>
+  </si>
+  <si>
+    <t>1.1.5.4</t>
+  </si>
+  <si>
+    <t>2.0.4.4</t>
+  </si>
+  <si>
+    <t>3.0.3.3</t>
+  </si>
+  <si>
+    <t>4.0.1.0</t>
+  </si>
+  <si>
+    <t>Hotfix Pull up en DCDC R22 y C11</t>
   </si>
 </sst>
 </file>
@@ -331,7 +347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +417,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,6 +639,15 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -653,19 +684,10 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -985,8 +1007,8 @@
   <dimension ref="A1:S100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <pane ySplit="10" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,56 +1036,56 @@
       <c r="A1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1072,41 +1094,41 @@
     </row>
     <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="39" t="s">
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="38" t="s">
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="33" t="s">
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="22" t="s">
         <v>23</v>
       </c>
@@ -1131,19 +1153,19 @@
       <c r="J9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="L9" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="42" t="s">
+      <c r="M9" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="N9" s="42" t="s">
+      <c r="N9" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="O9" s="42" t="s">
+      <c r="O9" s="23" t="s">
         <v>68</v>
       </c>
       <c r="P9" s="24" t="s">
@@ -1155,11 +1177,11 @@
       <c r="R9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="S9" s="34"/>
+      <c r="S9" s="37"/>
     </row>
     <row r="10" spans="1:19" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
-      <c r="B10" s="32"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="7">
         <f>MAX(C11:C37)</f>
         <v>125</v>
@@ -1178,7 +1200,7 @@
       </c>
       <c r="G10" s="8">
         <f>MAX(G11:G100)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" ref="H10:O10" si="1">MAX(H11:H100)</f>
@@ -1192,7 +1214,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K10" s="43">
+      <c r="K10" s="28">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1222,7 +1244,7 @@
       </c>
       <c r="R10" s="9">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S10" s="21"/>
     </row>
@@ -2060,7 +2082,7 @@
       <c r="S29" s="11"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="26" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2078,8 +2100,8 @@
       <c r="F30" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="20">
-        <v>7</v>
+      <c r="G30" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H30" s="20">
         <v>6</v>
@@ -2117,7 +2139,7 @@
       <c r="S30" s="11"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="26" t="s">
         <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2135,8 +2157,8 @@
       <c r="F31" s="20">
         <v>205</v>
       </c>
-      <c r="G31" s="20">
-        <v>7</v>
+      <c r="G31" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H31" s="20">
         <v>6</v>
@@ -2174,7 +2196,7 @@
       <c r="S31" s="11"/>
     </row>
     <row r="32" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2192,8 +2214,8 @@
       <c r="F32" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="20">
-        <v>7</v>
+      <c r="G32" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H32" s="20">
         <v>6</v>
@@ -2231,7 +2253,7 @@
       <c r="S32" s="11"/>
     </row>
     <row r="33" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="26" t="s">
         <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2249,8 +2271,8 @@
       <c r="F33" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="20">
-        <v>7</v>
+      <c r="G33" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H33" s="20">
         <v>6</v>
@@ -2287,94 +2309,232 @@
       </c>
       <c r="S33" s="11"/>
     </row>
-    <row r="34" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q34" s="6">
-        <v>10</v>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="29">
+        <v>8</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q34" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="R34" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S34" s="11"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
+      <c r="A35" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="29">
+        <v>8</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R35" s="6">
+        <v>13</v>
+      </c>
       <c r="S35" s="11"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
+      <c r="A36" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="29">
+        <v>8</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R36" s="6">
+        <v>13</v>
+      </c>
       <c r="S36" s="11"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
+      <c r="A37" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="29">
+        <v>8</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R37" s="6">
+        <v>13</v>
+      </c>
       <c r="S37" s="11"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>